<commit_message>
docs(us_5002): add self assessment
</commit_message>
<xml_diff>
--- a/docs/us_5002/Group-Evaluation.xlsx
+++ b/docs/us_5002/Group-Evaluation.xlsx
@@ -5,18 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\projects\sem4pi-22-23-9\docs\us_5002\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\sem4pi-22-23-9\docs\us_5002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616D7F7A-F591-4F75-8A44-1F4B908F5AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47575150-0356-439A-AE80-953F9436CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>options</t>
   </si>
@@ -70,9 +81,6 @@
   </si>
   <si>
     <t>João Teixeira</t>
-  </si>
-  <si>
-    <t>118----</t>
   </si>
   <si>
     <t>Jonas Antunes</t>
@@ -284,43 +292,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -457,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -755,257 +763,266 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="164" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="G2" s="8" t="s">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="G2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="G3" s="9" t="s">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="5" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="4"/>
+      <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="12" t="s">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="12" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C9" s="13">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="6">
         <v>1210957</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="13">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="6">
         <v>1210957</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <f>1181478</f>
+        <v>1181478</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="7">
+        <f>1181478</f>
+        <v>1181478</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="8">
+        <v>1211155</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="8">
+        <v>1211155</v>
+      </c>
+      <c r="M11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C11" s="15">
-        <v>1211155</v>
-      </c>
-      <c r="D11" s="1" t="s">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>1210951</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="16" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="7">
+        <v>1210951</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
+        <v>1210954</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="15">
-        <v>1211155</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C12" s="14">
-        <v>1210951</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="9">
+        <v>1210954</v>
+      </c>
+      <c r="M13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="14">
-        <v>1210951</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C13" s="17">
-        <v>1210954</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="17">
-        <v>1210954</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="M13:N13"/>
@@ -1022,9 +1039,6 @@
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:G13 O9:P13" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
docs(Group-Evaluation): added semester improvements
</commit_message>
<xml_diff>
--- a/docs/us_5002/Group-Evaluation.xlsx
+++ b/docs/us_5002/Group-Evaluation.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\sem4pi-22-23-9\docs\us_5002\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae2f95762269e7b3/Área de Trabalho/I.S.E.P/JOVAMI/sem4pi-22-23-9/docs/us_5002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47575150-0356-439A-AE80-953F9436CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{47575150-0356-439A-AE80-953F9436CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBE50D9C-1D60-493B-ABF9-DA55F61B0912}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>options</t>
   </si>
@@ -307,6 +307,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -326,9 +329,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,7 +764,7 @@
   <dimension ref="C2:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B5" zoomScale="164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,14 +777,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G3" s="5" t="s">
@@ -807,68 +807,68 @@
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15" t="s">
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11" t="s">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="11"/>
+      <c r="P7" s="12"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
       <c r="O8" s="2" t="s">
         <v>12</v>
       </c>
@@ -880,57 +880,61 @@
       <c r="C9" s="6">
         <v>1210957</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
       <c r="L9" s="6">
         <v>1210957</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="7">
         <f>1181478</f>
         <v>1181478</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="7">
         <f>1181478</f>
         <v>1181478</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="10"/>
+      <c r="N10" s="11"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
@@ -938,27 +942,27 @@
       <c r="C11" s="8">
         <v>1211155</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="8">
         <v>1211155</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="17"/>
+      <c r="N11" s="10"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
@@ -966,27 +970,27 @@
       <c r="C12" s="7">
         <v>1210951</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="7">
         <v>1210951</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="10"/>
+      <c r="N12" s="11"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
@@ -994,38 +998,32 @@
       <c r="C13" s="9">
         <v>1210954</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="9">
         <v>1210954</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="11"/>
+      <c r="N13" s="12"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="M13:N13"/>
     <mergeCell ref="G2:L2"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="H6:K6"/>
@@ -1039,6 +1037,12 @@
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="M10:N10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:G13 O9:P13" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>